<commit_message>
Updated XLS to 10 Samples
</commit_message>
<xml_diff>
--- a/Ajay Work/LF21 DOE.XLSX
+++ b/Ajay Work/LF21 DOE.XLSX
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="19160" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="19160" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LF21 FIREX DOE" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="44">
   <si>
     <t>Run</t>
   </si>
@@ -267,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,6 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1357,7 +1358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -2489,10 +2490,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="K1:O12"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2508,7 +2509,31 @@
     <col min="11" max="11" width="42.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="11:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
       <c r="L1" t="s">
         <v>26</v>
       </c>
@@ -2521,192 +2546,1083 @@
       <c r="O1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2500</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>-1.0263709779791299</v>
+      </c>
+      <c r="I2">
+        <v>0.48446431401864598</v>
+      </c>
       <c r="K2" t="s">
         <v>30</v>
       </c>
       <c r="L2">
-        <v>2.0648936340051601E-2</v>
+        <v>-0.22315477136481299</v>
       </c>
       <c r="M2">
-        <v>0.80346974475820399</v>
+        <v>0.190002091834892</v>
       </c>
       <c r="N2">
-        <v>2.5699706149191301E-2</v>
+        <v>-1.1744858659699899</v>
       </c>
       <c r="O2">
-        <v>0.97949685823963395</v>
-      </c>
-    </row>
-    <row r="3" spans="11:15" x14ac:dyDescent="0.35">
+        <v>0.240200469979509</v>
+      </c>
+      <c r="P2">
+        <v>0.61</v>
+      </c>
+      <c r="Q2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>2500</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>-1.0263709779791299</v>
+      </c>
+      <c r="I3">
+        <v>-0.78173934923713995</v>
+      </c>
       <c r="K3" t="s">
         <v>31</v>
       </c>
       <c r="L3">
-        <v>0.33921867561567498</v>
+        <v>0.89285828111301202</v>
       </c>
       <c r="M3">
-        <v>0.20334899403315301</v>
+        <v>0.20125949945457</v>
       </c>
       <c r="N3">
-        <v>1.6681600871867199</v>
-      </c>
-      <c r="O3">
-        <v>9.5283951722477306E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="11:15" x14ac:dyDescent="0.35">
+        <v>4.4363534816132004</v>
+      </c>
+      <c r="O3" s="10">
+        <v>9.1495560210486104E-6</v>
+      </c>
+      <c r="P3">
+        <v>0.78</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>-1.0263709779791299</v>
+      </c>
+      <c r="I4">
+        <v>0.28780708653718901</v>
+      </c>
       <c r="K4" t="s">
         <v>32</v>
       </c>
       <c r="L4">
-        <v>0.56535948077412501</v>
+        <v>0.47067959772153301</v>
       </c>
       <c r="M4">
-        <v>0.22325905271913399</v>
+        <v>0.22177213218365499</v>
       </c>
       <c r="N4">
-        <v>2.5323026049266799</v>
+        <v>2.1223568222347802</v>
       </c>
       <c r="O4">
-        <v>1.13316151912941E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="11:15" x14ac:dyDescent="0.35">
+        <v>3.3807785154355001E-2</v>
+      </c>
+      <c r="P4">
+        <v>0.84</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2500</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>-1.0263709779791299</v>
+      </c>
+      <c r="I5">
+        <v>1.1495929168399801</v>
+      </c>
       <c r="K5" t="s">
         <v>33</v>
       </c>
       <c r="L5">
-        <v>0.49849120038466599</v>
+        <v>0.55599138445261898</v>
       </c>
       <c r="M5">
-        <v>0.29170949977210098</v>
+        <v>0.27401365855697801</v>
       </c>
       <c r="N5">
-        <v>1.70886172981721</v>
+        <v>2.0290644903637398</v>
       </c>
       <c r="O5">
-        <v>8.7476564935182299E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="11:15" x14ac:dyDescent="0.35">
+        <v>4.2451722122188097E-2</v>
+      </c>
+      <c r="P5">
+        <v>0.63</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>7500</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>-1.0263709779791299</v>
+      </c>
+      <c r="I6">
+        <v>-1.4797300472080901</v>
+      </c>
       <c r="K6" t="s">
         <v>34</v>
       </c>
       <c r="L6">
-        <v>0.495151514690372</v>
+        <v>0.548940545563955</v>
       </c>
       <c r="M6">
-        <v>0.24990660147162</v>
+        <v>0.242928573825448</v>
       </c>
       <c r="N6">
-        <v>1.9813462780678199</v>
+        <v>2.2596787891999401</v>
       </c>
       <c r="O6">
-        <v>4.7552453909454701E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="11:15" x14ac:dyDescent="0.35">
+        <v>2.38411936580341E-2</v>
+      </c>
+      <c r="P6">
+        <v>0.73</v>
+      </c>
+      <c r="Q6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>-1.0263709779791299</v>
+      </c>
+      <c r="I7">
+        <v>-1.67772567098235</v>
+      </c>
       <c r="K7" t="s">
         <v>35</v>
       </c>
       <c r="L7">
-        <v>0.644422949822549</v>
+        <v>0.32805650458523899</v>
       </c>
       <c r="M7">
-        <v>0.31353040688061501</v>
+        <v>0.42228521358503102</v>
       </c>
       <c r="N7">
-        <v>2.05537624319778</v>
+        <v>0.776860032109986</v>
       </c>
       <c r="O7">
-        <v>3.9842678292325101E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="11:15" x14ac:dyDescent="0.35">
+        <v>0.437241353967529</v>
+      </c>
+      <c r="P7">
+        <v>0.66</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>2500</v>
+      </c>
+      <c r="E8">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>-1.0263709779791299</v>
+      </c>
+      <c r="I8">
+        <v>-0.30262004403838</v>
+      </c>
       <c r="K8" t="s">
         <v>36</v>
       </c>
       <c r="L8">
-        <v>0.34249768019207899</v>
+        <v>6.2665062495474901E-3</v>
       </c>
       <c r="M8">
-        <v>0.39017282539290599</v>
+        <v>0.38841441934308801</v>
       </c>
       <c r="N8">
-        <v>0.87781018538946698</v>
+        <v>1.6133557194261201E-2</v>
       </c>
       <c r="O8">
-        <v>0.38004673611060902</v>
-      </c>
-    </row>
-    <row r="9" spans="11:15" x14ac:dyDescent="0.35">
+        <v>0.98712784222552696</v>
+      </c>
+      <c r="P8">
+        <v>0.52</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>2500</v>
+      </c>
+      <c r="E9">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>-1.0263709779791299</v>
+      </c>
+      <c r="I9">
+        <v>0.710806147469635</v>
+      </c>
       <c r="K9" t="s">
         <v>37</v>
       </c>
       <c r="L9">
-        <v>0.67943261339199801</v>
+        <v>-0.38322496408357898</v>
       </c>
       <c r="M9">
-        <v>0.58455216903616303</v>
+        <v>0.57780618711804799</v>
       </c>
       <c r="N9">
-        <v>1.16231304814467</v>
+        <v>-0.66324136471263595</v>
       </c>
       <c r="O9">
-        <v>0.245108328376862</v>
-      </c>
-    </row>
-    <row r="10" spans="11:15" x14ac:dyDescent="0.35">
+        <v>0.50717598312227397</v>
+      </c>
+      <c r="P9">
+        <v>0.32</v>
+      </c>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>5000</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I10">
+        <v>-0.20927536732451099</v>
+      </c>
       <c r="K10" t="s">
         <v>38</v>
       </c>
       <c r="L10">
-        <v>0.93796323298636097</v>
+        <v>0.22201213975329701</v>
       </c>
       <c r="M10">
-        <v>0.44397386926982002</v>
+        <v>0.44021979675055101</v>
       </c>
       <c r="N10">
-        <v>2.1126541400487802</v>
+        <v>0.50432111729654905</v>
       </c>
       <c r="O10">
-        <v>3.4630381177934301E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="11:15" x14ac:dyDescent="0.35">
+        <v>0.61403574028494201</v>
+      </c>
+      <c r="P10">
+        <v>0.32</v>
+      </c>
+      <c r="Q10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>2500</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I11">
+        <v>-0.58430446464024099</v>
+      </c>
       <c r="K11" t="s">
         <v>39</v>
       </c>
       <c r="L11">
-        <v>1.3272590408787199</v>
+        <v>5.7937849771999797E-2</v>
       </c>
       <c r="M11">
-        <v>0.62551278129014298</v>
+        <v>0.62408539809214902</v>
       </c>
       <c r="N11">
-        <v>2.1218735740958001</v>
+        <v>9.2836413011933794E-2</v>
       </c>
       <c r="O11">
-        <v>3.3848356112391197E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="11:15" x14ac:dyDescent="0.35">
+        <v>0.92603352251346405</v>
+      </c>
+      <c r="P11">
+        <v>0.33</v>
+      </c>
+      <c r="Q11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>5000</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I12">
+        <v>1.47830148676017</v>
+      </c>
       <c r="K12" t="s">
         <v>40</v>
       </c>
       <c r="L12">
-        <v>0.58722048622550904</v>
+        <v>0.139133431634966</v>
       </c>
       <c r="M12">
-        <v>0.47996405537824799</v>
+        <v>0.467059805361971</v>
       </c>
       <c r="N12">
-        <v>1.22346763188909</v>
+        <v>0.297892111540487</v>
       </c>
       <c r="O12">
-        <v>0.22115312237665</v>
+        <v>0.76578550886164998</v>
+      </c>
+      <c r="P12">
+        <v>0.39</v>
+      </c>
+      <c r="Q12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>7500</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I13">
+        <v>0.67715995979089505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>2500</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I14">
+        <v>0.61888703070726903</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>7500</v>
+      </c>
+      <c r="E15">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I15">
+        <v>-0.99302622283981701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>7500</v>
+      </c>
+      <c r="E16">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I16">
+        <v>-0.56044538211779404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>5000</v>
+      </c>
+      <c r="E17">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I17">
+        <v>1.4422820987241001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>2500</v>
+      </c>
+      <c r="E18">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I18">
+        <v>0.32444677394633398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>5000</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I19">
+        <v>-2.3503785766515201E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>5000</v>
+      </c>
+      <c r="E20">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I20">
+        <v>-0.18772811712600199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>5000</v>
+      </c>
+      <c r="E21">
+        <v>45</v>
+      </c>
+      <c r="F21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I21">
+        <v>-0.58294857599701699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>7500</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I22">
+        <v>0.472259109770789</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>5000</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I23">
+        <v>-0.56656315628541298</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>2500</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I24">
+        <v>0.71347383776068796</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>7500</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I25">
+        <v>-0.238059992989713</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>5000</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I26">
+        <v>-0.79168936188026195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I27">
+        <v>-0.155705519349294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>2500</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I28">
+        <v>0.46579632338840599</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>2500</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I29">
+        <v>1.7829428064666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>7500</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>-0.68909247056939704</v>
+      </c>
+      <c r="I30">
+        <v>0.66409918799920498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated up to 100 samples
</commit_message>
<xml_diff>
--- a/Ajay Work/LF21 DOE.XLSX
+++ b/Ajay Work/LF21 DOE.XLSX
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="19160" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="19160" windowHeight="9780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LF21 FIREX DOE" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="44">
   <si>
     <t>Run</t>
   </si>
@@ -1358,12 +1358,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2492,7 +2493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -3632,10 +3633,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3649,7 +3650,1124 @@
     <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42.453125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2500</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>-0.81218244268330597</v>
+      </c>
+      <c r="I2">
+        <v>1.7030736317969499</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2">
+        <v>0.58644556757961097</v>
+      </c>
+      <c r="M2">
+        <v>0.24981812806551401</v>
+      </c>
+      <c r="N2">
+        <v>2.34749004053789</v>
+      </c>
+      <c r="O2">
+        <v>1.8900378440306301E-2</v>
+      </c>
+      <c r="P2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>2500</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>-0.81218244268330597</v>
+      </c>
+      <c r="I3">
+        <v>0.69118605399732802</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3">
+        <v>0.57967342799147803</v>
+      </c>
+      <c r="M3">
+        <v>0.38805473045934902</v>
+      </c>
+      <c r="N3">
+        <v>1.49379296911367</v>
+      </c>
+      <c r="O3">
+        <v>0.135229739789927</v>
+      </c>
+      <c r="P3">
+        <v>0.91</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>-0.81218244268330597</v>
+      </c>
+      <c r="I4">
+        <v>0.99688005885675002</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4">
+        <v>0.455922737718646</v>
+      </c>
+      <c r="M4">
+        <v>0.42760577866462102</v>
+      </c>
+      <c r="N4">
+        <v>1.06622211501083</v>
+      </c>
+      <c r="O4">
+        <v>0.28632324739197801</v>
+      </c>
+      <c r="P4">
+        <v>0.79</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2500</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>-0.81218244268330597</v>
+      </c>
+      <c r="I5">
+        <v>1.6927958192435599</v>
+      </c>
+      <c r="K5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5">
+        <v>-2.04383539041419E-2</v>
+      </c>
+      <c r="M5">
+        <v>0.52833429826506395</v>
+      </c>
+      <c r="N5">
+        <v>-3.8684510869835702E-2</v>
+      </c>
+      <c r="O5">
+        <v>0.96914192270108701</v>
+      </c>
+      <c r="P5">
+        <v>0.74</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>7500</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>-0.81218244268330597</v>
+      </c>
+      <c r="I6">
+        <v>0.25524911452487198</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6">
+        <v>-3.6504321135133203E-2</v>
+      </c>
+      <c r="M6">
+        <v>0.46839817495415897</v>
+      </c>
+      <c r="N6">
+        <v>-7.7934379523801195E-2</v>
+      </c>
+      <c r="O6">
+        <v>0.93788025166262601</v>
+      </c>
+      <c r="P6">
+        <v>0.71</v>
+      </c>
+      <c r="Q6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>-0.81218244268330597</v>
+      </c>
+      <c r="I7">
+        <v>-2.8861825847582399</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7">
+        <v>-0.365612060220531</v>
+      </c>
+      <c r="M7">
+        <v>0.612981620820512</v>
+      </c>
+      <c r="N7">
+        <v>-0.59644865001194902</v>
+      </c>
+      <c r="O7">
+        <v>0.55087554828268404</v>
+      </c>
+      <c r="P7">
+        <v>0.59</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>2500</v>
+      </c>
+      <c r="E8">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>-0.81218244268330597</v>
+      </c>
+      <c r="I8">
+        <v>0.49648999852154102</v>
+      </c>
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8">
+        <v>0.64395668926520599</v>
+      </c>
+      <c r="M8">
+        <v>0.74891398027515099</v>
+      </c>
+      <c r="N8">
+        <v>0.85985401024109098</v>
+      </c>
+      <c r="O8">
+        <v>0.38986952243830703</v>
+      </c>
+      <c r="P8">
+        <v>0.44</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>2500</v>
+      </c>
+      <c r="E9">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>-0.81218244268330597</v>
+      </c>
+      <c r="I9">
+        <v>-0.67026458454018301</v>
+      </c>
+      <c r="K9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9">
+        <v>1.2174405030925499</v>
+      </c>
+      <c r="M9">
+        <v>1.1140861664045401</v>
+      </c>
+      <c r="N9">
+        <v>1.0927705053744301</v>
+      </c>
+      <c r="O9">
+        <v>0.27449457463354099</v>
+      </c>
+      <c r="P9">
+        <v>0.33</v>
+      </c>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>5000</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I10">
+        <v>0.60638227013168</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10">
+        <v>-0.20827604621326201</v>
+      </c>
+      <c r="M10">
+        <v>0.84880154742442504</v>
+      </c>
+      <c r="N10">
+        <v>-0.24537660993343899</v>
+      </c>
+      <c r="O10">
+        <v>0.80616483807100303</v>
+      </c>
+      <c r="P10">
+        <v>0.39</v>
+      </c>
+      <c r="Q10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>2500</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I11">
+        <v>-1.9529837310463201</v>
+      </c>
+      <c r="K11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11">
+        <v>0.41562180651180303</v>
+      </c>
+      <c r="M11">
+        <v>1.2033185593554101</v>
+      </c>
+      <c r="N11">
+        <v>0.34539632359235101</v>
+      </c>
+      <c r="O11">
+        <v>0.72979644066411498</v>
+      </c>
+      <c r="P11">
+        <v>0.32</v>
+      </c>
+      <c r="Q11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>5000</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I12">
+        <v>1.4832641365455299</v>
+      </c>
+      <c r="K12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12">
+        <v>0.117107821925629</v>
+      </c>
+      <c r="M12">
+        <v>0.90055260680526406</v>
+      </c>
+      <c r="N12">
+        <v>0.13003995662293599</v>
+      </c>
+      <c r="O12">
+        <v>0.89653481425798998</v>
+      </c>
+      <c r="P12">
+        <v>0.45</v>
+      </c>
+      <c r="Q12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>7500</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I13">
+        <v>0.82845571518222305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>2500</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I14">
+        <v>1.17942876910367</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>7500</v>
+      </c>
+      <c r="E15">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I15">
+        <v>0.81031924320205095</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>7500</v>
+      </c>
+      <c r="E16">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I16">
+        <v>-0.19934722198270599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>5000</v>
+      </c>
+      <c r="E17">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I17">
+        <v>0.86033634670667902</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>2500</v>
+      </c>
+      <c r="E18">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I18">
+        <v>-1.4223739309425201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>5000</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I19">
+        <v>0.37306227824341098</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>5000</v>
+      </c>
+      <c r="E20">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I20">
+        <v>0.63954336332922102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>5000</v>
+      </c>
+      <c r="E21">
+        <v>45</v>
+      </c>
+      <c r="F21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I21">
+        <v>-0.25950755925075197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>7500</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I22">
+        <v>-0.145099634574724</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>5000</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I23">
+        <v>1.4678672754191699</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>2500</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I24">
+        <v>-0.52901689205168601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>7500</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I25">
+        <v>-8.7945411630587E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>5000</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I26">
+        <v>-1.92721299046048</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I27">
+        <v>-0.93379615062732602</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>2500</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I28">
+        <v>1.30045869196953</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>2500</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I29">
+        <v>-0.62866822604994399</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>7500</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>-2.6715352610625702</v>
+      </c>
+      <c r="I30">
+        <v>-2.5870679897845101</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated to 1000 samples and fixed glitches
Ran the code for 1000 simulations and also fixed glitches that were discussed with Ray
</commit_message>
<xml_diff>
--- a/Ajay Work/LF21 DOE.XLSX
+++ b/Ajay Work/LF21 DOE.XLSX
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="19160" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="19160" windowHeight="9780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LF21 FIREX DOE" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LF21 FIREX DOE'!$B$2:$G$32</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="44">
   <si>
     <t>Run</t>
   </si>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2493,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="C1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2574,31 +2574,31 @@
         <v>41</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>-1.0263709779791299</v>
+        <v>-1.0816751645219</v>
       </c>
       <c r="I2">
-        <v>0.48446431401864598</v>
+        <v>-0.34420589879929703</v>
       </c>
       <c r="K2" t="s">
         <v>30</v>
       </c>
       <c r="L2">
-        <v>-0.22315477136481299</v>
+        <v>0.15352800971451999</v>
       </c>
       <c r="M2">
-        <v>0.190002091834892</v>
+        <v>0.447377715169333</v>
       </c>
       <c r="N2">
-        <v>-1.1744858659699899</v>
+        <v>0.34317312755824098</v>
       </c>
       <c r="O2">
-        <v>0.240200469979509</v>
+        <v>0.73146821960790698</v>
       </c>
       <c r="P2">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
       <c r="Q2">
         <v>100</v>
@@ -2624,31 +2624,31 @@
         <v>41</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>-1.0263709779791299</v>
+        <v>-1.0816751645219</v>
       </c>
       <c r="I3">
-        <v>-0.78173934923713995</v>
+        <v>0.98999324604773797</v>
       </c>
       <c r="K3" t="s">
         <v>31</v>
       </c>
       <c r="L3">
-        <v>0.89285828111301202</v>
+        <v>0.68537534608056505</v>
       </c>
       <c r="M3">
-        <v>0.20125949945457</v>
+        <v>0.24475908078160599</v>
       </c>
       <c r="N3">
-        <v>4.4363534816132004</v>
-      </c>
-      <c r="O3" s="10">
-        <v>9.1495560210486104E-6</v>
+        <v>2.8002039552195899</v>
+      </c>
+      <c r="O3">
+        <v>5.10703278731284E-3</v>
       </c>
       <c r="P3">
-        <v>0.78</v>
+        <v>0.74</v>
       </c>
       <c r="Q3">
         <v>100</v>
@@ -2674,31 +2674,31 @@
         <v>41</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>-1.0263709779791299</v>
+        <v>-1.0816751645219</v>
       </c>
       <c r="I4">
-        <v>0.28780708653718901</v>
+        <v>0.188239703011577</v>
       </c>
       <c r="K4" t="s">
         <v>32</v>
       </c>
       <c r="L4">
-        <v>0.47067959772153301</v>
+        <v>0.33962309603267299</v>
       </c>
       <c r="M4">
-        <v>0.22177213218365499</v>
+        <v>0.28314092113089101</v>
       </c>
       <c r="N4">
-        <v>2.1223568222347802</v>
+        <v>1.19948432277534</v>
       </c>
       <c r="O4">
-        <v>3.3807785154355001E-2</v>
+        <v>0.23033967706536801</v>
       </c>
       <c r="P4">
-        <v>0.84</v>
+        <v>0.76</v>
       </c>
       <c r="Q4">
         <v>100</v>
@@ -2724,31 +2724,31 @@
         <v>41</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>-1.0263709779791299</v>
+        <v>-1.0816751645219</v>
       </c>
       <c r="I5">
-        <v>1.1495929168399801</v>
+        <v>0.87849553881586295</v>
       </c>
       <c r="K5" t="s">
         <v>33</v>
       </c>
       <c r="L5">
-        <v>0.55599138445261898</v>
+        <v>-0.139940555764343</v>
       </c>
       <c r="M5">
-        <v>0.27401365855697801</v>
+        <v>0.32864335375269399</v>
       </c>
       <c r="N5">
-        <v>2.0290644903637398</v>
+        <v>-0.42581282769420897</v>
       </c>
       <c r="O5">
-        <v>4.2451722122188097E-2</v>
+        <v>0.67024423896849605</v>
       </c>
       <c r="P5">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="Q5">
         <v>100</v>
@@ -2777,28 +2777,28 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>-1.0263709779791299</v>
+        <v>-1.0816751645219</v>
       </c>
       <c r="I6">
-        <v>-1.4797300472080901</v>
+        <v>-0.25846624673635799</v>
       </c>
       <c r="K6" t="s">
         <v>34</v>
       </c>
       <c r="L6">
-        <v>0.548940545563955</v>
+        <v>0.58691341463364199</v>
       </c>
       <c r="M6">
-        <v>0.242928573825448</v>
+        <v>0.291332768463827</v>
       </c>
       <c r="N6">
-        <v>2.2596787891999401</v>
+        <v>2.0145808441954101</v>
       </c>
       <c r="O6">
-        <v>2.38411936580341E-2</v>
+        <v>4.3948586266751903E-2</v>
       </c>
       <c r="P6">
-        <v>0.73</v>
+        <v>0.76</v>
       </c>
       <c r="Q6">
         <v>100</v>
@@ -2824,31 +2824,31 @@
         <v>41</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>-1.0263709779791299</v>
+        <v>-1.0816751645219</v>
       </c>
       <c r="I7">
-        <v>-1.67772567098235</v>
+        <v>0.99222610742580197</v>
       </c>
       <c r="K7" t="s">
         <v>35</v>
       </c>
       <c r="L7">
-        <v>0.32805650458523899</v>
+        <v>0.68590399489005804</v>
       </c>
       <c r="M7">
-        <v>0.42228521358503102</v>
+        <v>0.38714509291829902</v>
       </c>
       <c r="N7">
-        <v>0.776860032109986</v>
+        <v>1.7716975042088601</v>
       </c>
       <c r="O7">
-        <v>0.437241353967529</v>
+        <v>7.6444784187812198E-2</v>
       </c>
       <c r="P7">
-        <v>0.66</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q7">
         <v>100</v>
@@ -2877,28 +2877,28 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>-1.0263709779791299</v>
+        <v>-1.0816751645219</v>
       </c>
       <c r="I8">
-        <v>-0.30262004403838</v>
+        <v>-1.52297664111903</v>
       </c>
       <c r="K8" t="s">
         <v>36</v>
       </c>
       <c r="L8">
-        <v>6.2665062495474901E-3</v>
+        <v>0.121413155396904</v>
       </c>
       <c r="M8">
-        <v>0.38841441934308801</v>
+        <v>0.47452782144592098</v>
       </c>
       <c r="N8">
-        <v>1.6133557194261201E-2</v>
+        <v>0.25586098413987401</v>
       </c>
       <c r="O8">
-        <v>0.98712784222552696</v>
+        <v>0.79805818215598101</v>
       </c>
       <c r="P8">
-        <v>0.52</v>
+        <v>0.36</v>
       </c>
       <c r="Q8">
         <v>100</v>
@@ -2927,28 +2927,28 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>-1.0263709779791299</v>
+        <v>-1.0816751645219</v>
       </c>
       <c r="I9">
-        <v>0.710806147469635</v>
+        <v>0.46851301242814403</v>
       </c>
       <c r="K9" t="s">
         <v>37</v>
       </c>
       <c r="L9">
-        <v>-0.38322496408357898</v>
+        <v>0.39838530720384602</v>
       </c>
       <c r="M9">
-        <v>0.57780618711804799</v>
+        <v>0.71490613225354205</v>
       </c>
       <c r="N9">
-        <v>-0.66324136471263595</v>
+        <v>0.55725540631194104</v>
       </c>
       <c r="O9">
-        <v>0.50717598312227397</v>
+        <v>0.57735293897559603</v>
       </c>
       <c r="P9">
-        <v>0.32</v>
+        <v>0.35</v>
       </c>
       <c r="Q9">
         <v>100</v>
@@ -2974,31 +2974,31 @@
         <v>41</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I10">
-        <v>-0.20927536732451099</v>
+        <v>0.94630232137902104</v>
       </c>
       <c r="K10" t="s">
         <v>38</v>
       </c>
       <c r="L10">
-        <v>0.22201213975329701</v>
+        <v>1.17976979045354</v>
       </c>
       <c r="M10">
-        <v>0.44021979675055101</v>
+        <v>0.58926525212003</v>
       </c>
       <c r="N10">
-        <v>0.50432111729654905</v>
+        <v>2.00210310417765</v>
       </c>
       <c r="O10">
-        <v>0.61403574028494201</v>
+        <v>4.527364374903E-2</v>
       </c>
       <c r="P10">
-        <v>0.32</v>
+        <v>0.37</v>
       </c>
       <c r="Q10">
         <v>100</v>
@@ -3024,31 +3024,31 @@
         <v>41</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I11">
-        <v>-0.58430446464024099</v>
+        <v>-1.9397158751195001</v>
       </c>
       <c r="K11" t="s">
         <v>39</v>
       </c>
       <c r="L11">
-        <v>5.7937849771999797E-2</v>
+        <v>0.60136945703594402</v>
       </c>
       <c r="M11">
-        <v>0.62408539809214902</v>
+        <v>0.76878589547311504</v>
       </c>
       <c r="N11">
-        <v>9.2836413011933794E-2</v>
+        <v>0.78223268738022</v>
       </c>
       <c r="O11">
-        <v>0.92603352251346405</v>
+        <v>0.43407783766767799</v>
       </c>
       <c r="P11">
-        <v>0.33</v>
+        <v>0.43</v>
       </c>
       <c r="Q11">
         <v>100</v>
@@ -3077,28 +3077,28 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I12">
-        <v>1.47830148676017</v>
+        <v>-0.115596046729457</v>
       </c>
       <c r="K12" t="s">
         <v>40</v>
       </c>
       <c r="L12">
-        <v>0.139133431634966</v>
+        <v>-0.99239711333771496</v>
       </c>
       <c r="M12">
-        <v>0.467059805361971</v>
+        <v>0.57274944763161595</v>
       </c>
       <c r="N12">
-        <v>0.297892111540487</v>
+        <v>-1.7326897781244299</v>
       </c>
       <c r="O12">
-        <v>0.76578550886164998</v>
+        <v>8.3150822321207907E-2</v>
       </c>
       <c r="P12">
-        <v>0.39</v>
+        <v>0.5</v>
       </c>
       <c r="Q12">
         <v>100</v>
@@ -3124,13 +3124,13 @@
         <v>41</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I13">
-        <v>0.67715995979089505</v>
+        <v>0.88355694808381102</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
@@ -3156,10 +3156,10 @@
         <v>2</v>
       </c>
       <c r="H14">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I14">
-        <v>0.61888703070726903</v>
+        <v>-0.64742642704581199</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
@@ -3185,10 +3185,10 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I15">
-        <v>-0.99302622283981701</v>
+        <v>3.5173317231852699E-2</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
@@ -3211,13 +3211,13 @@
         <v>41</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I16">
-        <v>-0.56044538211779404</v>
+        <v>0.72076643770354298</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -3240,13 +3240,13 @@
         <v>41</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I17">
-        <v>1.4422820987241001</v>
+        <v>-0.37636315697862499</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -3269,13 +3269,13 @@
         <v>41</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I18">
-        <v>0.32444677394633398</v>
+        <v>1.1489762096943501</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -3301,10 +3301,10 @@
         <v>2</v>
       </c>
       <c r="H19">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I19">
-        <v>-2.3503785766515201E-2</v>
+        <v>-0.298008288373105</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -3330,10 +3330,10 @@
         <v>1</v>
       </c>
       <c r="H20">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I20">
-        <v>-0.18772811712600199</v>
+        <v>1.2250347681476501</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -3356,13 +3356,13 @@
         <v>41</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H21">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I21">
-        <v>-0.58294857599701699</v>
+        <v>0.43827399059069899</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -3388,10 +3388,10 @@
         <v>2</v>
       </c>
       <c r="H22">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I22">
-        <v>0.472259109770789</v>
+        <v>-1.2523481604956499</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -3417,10 +3417,10 @@
         <v>2</v>
       </c>
       <c r="H23">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I23">
-        <v>-0.56656315628541298</v>
+        <v>-1.8582031806592001</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -3446,10 +3446,10 @@
         <v>2</v>
       </c>
       <c r="H24">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I24">
-        <v>0.71347383776068796</v>
+        <v>0.28133589331501802</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -3475,10 +3475,10 @@
         <v>2</v>
       </c>
       <c r="H25">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I25">
-        <v>-0.238059992989713</v>
+        <v>-0.766959883197603</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -3504,10 +3504,10 @@
         <v>2</v>
       </c>
       <c r="H26">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I26">
-        <v>-0.79168936188026195</v>
+        <v>-0.57617914372005496</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -3533,10 +3533,10 @@
         <v>2</v>
       </c>
       <c r="H27">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I27">
-        <v>-0.155705519349294</v>
+        <v>-0.72861782367873196</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -3562,10 +3562,10 @@
         <v>2</v>
       </c>
       <c r="H28">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I28">
-        <v>0.46579632338840599</v>
+        <v>0.59769989997587702</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -3591,10 +3591,10 @@
         <v>2</v>
       </c>
       <c r="H29">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I29">
-        <v>1.7829428064666</v>
+        <v>-0.16064906082873201</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -3620,10 +3620,10 @@
         <v>2</v>
       </c>
       <c r="H30">
-        <v>-0.68909247056939704</v>
+        <v>1.2890320243156199</v>
       </c>
       <c r="I30">
-        <v>0.66409918799920498</v>
+        <v>-0.25432046086421101</v>
       </c>
     </row>
   </sheetData>
@@ -3635,8 +3635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3718,28 +3718,28 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>-0.81218244268330597</v>
+        <v>-1.2398397779972601</v>
       </c>
       <c r="I2">
-        <v>1.7030736317969499</v>
+        <v>0.73982636523197198</v>
       </c>
       <c r="K2" t="s">
         <v>30</v>
       </c>
       <c r="L2">
-        <v>0.58644556757961097</v>
+        <v>-0.290187539216195</v>
       </c>
       <c r="M2">
-        <v>0.24981812806551401</v>
+        <v>8.76452445593843E-2</v>
       </c>
       <c r="N2">
-        <v>2.34749004053789</v>
+        <v>-3.3109330765752798</v>
       </c>
       <c r="O2">
-        <v>1.8900378440306301E-2</v>
+        <v>9.2985443829718395E-4</v>
       </c>
       <c r="P2">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="Q2">
         <v>100</v>
@@ -3765,31 +3765,31 @@
         <v>41</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>-0.81218244268330597</v>
+        <v>-1.2398397779972601</v>
       </c>
       <c r="I3">
-        <v>0.69118605399732802</v>
+        <v>2.1108032953912899</v>
       </c>
       <c r="K3" t="s">
         <v>31</v>
       </c>
       <c r="L3">
-        <v>0.57967342799147803</v>
+        <v>0.65995624535129205</v>
       </c>
       <c r="M3">
-        <v>0.38805473045934902</v>
+        <v>0.14558025926197801</v>
       </c>
       <c r="N3">
-        <v>1.49379296911367</v>
-      </c>
-      <c r="O3">
-        <v>0.135229739789927</v>
+        <v>4.5332811515582696</v>
+      </c>
+      <c r="O3" s="10">
+        <v>5.8074432576216097E-6</v>
       </c>
       <c r="P3">
-        <v>0.91</v>
+        <v>0.82</v>
       </c>
       <c r="Q3">
         <v>100</v>
@@ -3815,31 +3815,31 @@
         <v>41</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>-0.81218244268330597</v>
+        <v>-1.2398397779972601</v>
       </c>
       <c r="I4">
-        <v>0.99688005885675002</v>
+        <v>0.77329502180310195</v>
       </c>
       <c r="K4" t="s">
         <v>32</v>
       </c>
       <c r="L4">
-        <v>0.455922737718646</v>
+        <v>1.1119002234522499</v>
       </c>
       <c r="M4">
-        <v>0.42760577866462102</v>
+        <v>0.16041799064329801</v>
       </c>
       <c r="N4">
-        <v>1.06622211501083</v>
-      </c>
-      <c r="O4">
-        <v>0.28632324739197801</v>
+        <v>6.93126886201091</v>
+      </c>
+      <c r="O4" s="10">
+        <v>4.1708858589117897E-12</v>
       </c>
       <c r="P4">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
       <c r="Q4">
         <v>100</v>
@@ -3868,28 +3868,28 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>-0.81218244268330597</v>
+        <v>-1.2398397779972601</v>
       </c>
       <c r="I5">
-        <v>1.6927958192435599</v>
+        <v>0.158376572774617</v>
       </c>
       <c r="K5" t="s">
         <v>33</v>
       </c>
       <c r="L5">
-        <v>-2.04383539041419E-2</v>
+        <v>0.25682880950806902</v>
       </c>
       <c r="M5">
-        <v>0.52833429826506395</v>
+        <v>0.19820669117311701</v>
       </c>
       <c r="N5">
-        <v>-3.8684510869835702E-2</v>
+        <v>1.2957625597197999</v>
       </c>
       <c r="O5">
-        <v>0.96914192270108701</v>
+        <v>0.195057300712248</v>
       </c>
       <c r="P5">
-        <v>0.74</v>
+        <v>0.61</v>
       </c>
       <c r="Q5">
         <v>100</v>
@@ -3918,28 +3918,28 @@
         <v>2</v>
       </c>
       <c r="H6">
-        <v>-0.81218244268330597</v>
+        <v>-1.2398397779972601</v>
       </c>
       <c r="I6">
-        <v>0.25524911452487198</v>
+        <v>-0.87782535545804696</v>
       </c>
       <c r="K6" t="s">
         <v>34</v>
       </c>
       <c r="L6">
-        <v>-3.6504321135133203E-2</v>
+        <v>0.44496244741762903</v>
       </c>
       <c r="M6">
-        <v>0.46839817495415897</v>
+        <v>0.175721418643567</v>
       </c>
       <c r="N6">
-        <v>-7.7934379523801195E-2</v>
+        <v>2.53220381927482</v>
       </c>
       <c r="O6">
-        <v>0.93788025166262601</v>
+        <v>1.1334808341179701E-2</v>
       </c>
       <c r="P6">
-        <v>0.71</v>
+        <v>0.77</v>
       </c>
       <c r="Q6">
         <v>100</v>
@@ -3965,31 +3965,31 @@
         <v>41</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>-0.81218244268330597</v>
+        <v>-1.2398397779972601</v>
       </c>
       <c r="I7">
-        <v>-2.8861825847582399</v>
+        <v>1.75391520814841</v>
       </c>
       <c r="K7" t="s">
         <v>35</v>
       </c>
       <c r="L7">
-        <v>-0.365612060220531</v>
+        <v>0.89998502940268299</v>
       </c>
       <c r="M7">
-        <v>0.612981620820512</v>
+        <v>0.220171633108246</v>
       </c>
       <c r="N7">
-        <v>-0.59644865001194902</v>
-      </c>
-      <c r="O7">
-        <v>0.55087554828268404</v>
+        <v>4.0876520589744301</v>
+      </c>
+      <c r="O7" s="10">
+        <v>4.3576105172027402E-5</v>
       </c>
       <c r="P7">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="Q7">
         <v>100</v>
@@ -4015,28 +4015,28 @@
         <v>41</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>-0.81218244268330597</v>
+        <v>-1.2398397779972601</v>
       </c>
       <c r="I8">
-        <v>0.49648999852154102</v>
+        <v>0.58979052331349502</v>
       </c>
       <c r="K8" t="s">
         <v>36</v>
       </c>
       <c r="L8">
-        <v>0.64395668926520599</v>
+        <v>0.574001014824147</v>
       </c>
       <c r="M8">
-        <v>0.74891398027515099</v>
+        <v>0.280958026936867</v>
       </c>
       <c r="N8">
-        <v>0.85985401024109098</v>
+        <v>2.04301340339754</v>
       </c>
       <c r="O8">
-        <v>0.38986952243830703</v>
+        <v>4.1051111307629097E-2</v>
       </c>
       <c r="P8">
         <v>0.44</v>
@@ -4065,31 +4065,31 @@
         <v>41</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>-0.81218244268330597</v>
+        <v>-1.2398397779972601</v>
       </c>
       <c r="I9">
-        <v>-0.67026458454018301</v>
+        <v>-1.3577584803643901</v>
       </c>
       <c r="K9" t="s">
         <v>37</v>
       </c>
       <c r="L9">
-        <v>1.2174405030925499</v>
+        <v>-0.35508482727952301</v>
       </c>
       <c r="M9">
-        <v>1.1140861664045401</v>
+        <v>0.41795380964270001</v>
       </c>
       <c r="N9">
-        <v>1.0927705053744301</v>
+        <v>-0.84957911397691899</v>
       </c>
       <c r="O9">
-        <v>0.27449457463354099</v>
+        <v>0.39555912800696502</v>
       </c>
       <c r="P9">
-        <v>0.33</v>
+        <v>0.36</v>
       </c>
       <c r="Q9">
         <v>100</v>
@@ -4115,31 +4115,31 @@
         <v>41</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I10">
-        <v>0.60638227013168</v>
+        <v>8.1380961692928494E-2</v>
       </c>
       <c r="K10" t="s">
         <v>38</v>
       </c>
       <c r="L10">
-        <v>-0.20827604621326201</v>
+        <v>0.67916124281553703</v>
       </c>
       <c r="M10">
-        <v>0.84880154742442504</v>
+        <v>0.31843124084518898</v>
       </c>
       <c r="N10">
-        <v>-0.24537660993343899</v>
+        <v>2.1328348343362502</v>
       </c>
       <c r="O10">
-        <v>0.80616483807100303</v>
+        <v>3.2938277592384803E-2</v>
       </c>
       <c r="P10">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="Q10">
         <v>100</v>
@@ -4168,28 +4168,28 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I11">
-        <v>-1.9529837310463201</v>
+        <v>0.32854858356739097</v>
       </c>
       <c r="K11" t="s">
         <v>39</v>
       </c>
       <c r="L11">
-        <v>0.41562180651180303</v>
+        <v>0.43419637146630702</v>
       </c>
       <c r="M11">
-        <v>1.2033185593554101</v>
+        <v>0.45142969301868002</v>
       </c>
       <c r="N11">
-        <v>0.34539632359235101</v>
+        <v>0.96182501545891796</v>
       </c>
       <c r="O11">
-        <v>0.72979644066411498</v>
+        <v>0.336137509969127</v>
       </c>
       <c r="P11">
-        <v>0.32</v>
+        <v>0.36</v>
       </c>
       <c r="Q11">
         <v>100</v>
@@ -4215,31 +4215,31 @@
         <v>41</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I12">
-        <v>1.4832641365455299</v>
+        <v>0.59863534902732896</v>
       </c>
       <c r="K12" t="s">
         <v>40</v>
       </c>
       <c r="L12">
-        <v>0.117107821925629</v>
+        <v>-0.430255278118722</v>
       </c>
       <c r="M12">
-        <v>0.90055260680526406</v>
+        <v>0.33784585443030501</v>
       </c>
       <c r="N12">
-        <v>0.13003995662293599</v>
+        <v>-1.27352540360231</v>
       </c>
       <c r="O12">
-        <v>0.89653481425798998</v>
+        <v>0.20283166393867499</v>
       </c>
       <c r="P12">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="Q12">
         <v>100</v>
@@ -4265,13 +4265,13 @@
         <v>41</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I13">
-        <v>0.82845571518222305</v>
+        <v>-0.26983562259764199</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
@@ -4294,13 +4294,13 @@
         <v>41</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I14">
-        <v>1.17942876910367</v>
+        <v>0.134538705752518</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
@@ -4323,13 +4323,13 @@
         <v>41</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I15">
-        <v>0.81031924320205095</v>
+        <v>0.197519480991384</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
@@ -4352,13 +4352,13 @@
         <v>41</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I16">
-        <v>-0.19934722198270599</v>
+        <v>-0.44695782358004099</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -4381,13 +4381,13 @@
         <v>41</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I17">
-        <v>0.86033634670667902</v>
+        <v>-1.04894638419913</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -4413,10 +4413,10 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I18">
-        <v>-1.4223739309425201</v>
+        <v>-0.12791705153388599</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -4442,10 +4442,10 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I19">
-        <v>0.37306227824341098</v>
+        <v>-0.56752110158180002</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -4471,10 +4471,10 @@
         <v>1</v>
       </c>
       <c r="H20">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I20">
-        <v>0.63954336332922102</v>
+        <v>0.25064506041512502</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -4500,10 +4500,10 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I21">
-        <v>-0.25950755925075197</v>
+        <v>2.0347183707560101</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -4529,10 +4529,10 @@
         <v>2</v>
       </c>
       <c r="H22">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I22">
-        <v>-0.145099634574724</v>
+        <v>2.02904216288043E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -4558,10 +4558,10 @@
         <v>2</v>
       </c>
       <c r="H23">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I23">
-        <v>1.4678672754191699</v>
+        <v>-0.50832292155225001</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -4587,10 +4587,10 @@
         <v>2</v>
       </c>
       <c r="H24">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I24">
-        <v>-0.52901689205168601</v>
+        <v>0.14959581644867001</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -4616,10 +4616,10 @@
         <v>2</v>
       </c>
       <c r="H25">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I25">
-        <v>-8.7945411630587E-2</v>
+        <v>-0.31512315038994299</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -4645,10 +4645,10 @@
         <v>2</v>
       </c>
       <c r="H26">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I26">
-        <v>-1.92721299046048</v>
+        <v>1.2638087572204899</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -4674,10 +4674,10 @@
         <v>2</v>
       </c>
       <c r="H27">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I27">
-        <v>-0.93379615062732602</v>
+        <v>4.2926253142760898E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -4703,10 +4703,10 @@
         <v>2</v>
       </c>
       <c r="H28">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I28">
-        <v>1.30045869196953</v>
+        <v>-0.90962233483735699</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -4732,10 +4732,10 @@
         <v>2</v>
       </c>
       <c r="H29">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I29">
-        <v>-0.62866822604994399</v>
+        <v>1.4832278850437699</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -4761,10 +4761,10 @@
         <v>2</v>
       </c>
       <c r="H30">
-        <v>-2.6715352610625702</v>
+        <v>0.76002991906394601</v>
       </c>
       <c r="I30">
-        <v>-2.5870679897845101</v>
+        <v>-0.71877919141094504</v>
       </c>
     </row>
   </sheetData>
@@ -4774,12 +4774,1134 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="11" max="11" width="42.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2500</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.31020527703066397</v>
+      </c>
+      <c r="I2">
+        <v>0.53628428276515505</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2">
+        <v>0.58842661266338303</v>
+      </c>
+      <c r="M2">
+        <v>0.33500627399286198</v>
+      </c>
+      <c r="N2">
+        <v>1.7564644555758999</v>
+      </c>
+      <c r="O2">
+        <v>7.9009135468894001E-2</v>
+      </c>
+      <c r="P2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>2500</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0.31020527703066397</v>
+      </c>
+      <c r="I3">
+        <v>-1.70959629843632</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3">
+        <v>0.63616736348847702</v>
+      </c>
+      <c r="M3">
+        <v>0.19286427464171699</v>
+      </c>
+      <c r="N3">
+        <v>3.29852361029684</v>
+      </c>
+      <c r="O3">
+        <v>9.7194705975600605E-4</v>
+      </c>
+      <c r="P3">
+        <v>0.85</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0.31020527703066397</v>
+      </c>
+      <c r="I4">
+        <v>1.01872680772141</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4">
+        <v>0.82296439143148503</v>
+      </c>
+      <c r="M4">
+        <v>0.21564620356387401</v>
+      </c>
+      <c r="N4">
+        <v>3.8162711785822201</v>
+      </c>
+      <c r="O4">
+        <v>1.3548360046944399E-4</v>
+      </c>
+      <c r="P4">
+        <v>0.84</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2500</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>0.31020527703066397</v>
+      </c>
+      <c r="I5">
+        <v>-0.17658320234175601</v>
+      </c>
+      <c r="K5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5">
+        <v>0.56431729801721997</v>
+      </c>
+      <c r="M5">
+        <v>0.26697103497249502</v>
+      </c>
+      <c r="N5">
+        <v>2.1137772420718202</v>
+      </c>
+      <c r="O5">
+        <v>3.45342976063314E-2</v>
+      </c>
+      <c r="P5">
+        <v>0.69</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>7500</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0.31020527703066397</v>
+      </c>
+      <c r="I6">
+        <v>0.78812127684411803</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6">
+        <v>0.52570271960666803</v>
+      </c>
+      <c r="M6">
+        <v>0.25365038529546602</v>
+      </c>
+      <c r="N6">
+        <v>2.0725484764957098</v>
+      </c>
+      <c r="O6">
+        <v>3.8214320323948003E-2</v>
+      </c>
+      <c r="P6">
+        <v>0.74</v>
+      </c>
+      <c r="Q6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.31020527703066397</v>
+      </c>
+      <c r="I7">
+        <v>2.4226635714065399</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7">
+        <v>0.68484141249393304</v>
+      </c>
+      <c r="M7">
+        <v>0.40069076092127598</v>
+      </c>
+      <c r="N7">
+        <v>1.7091519927220999</v>
+      </c>
+      <c r="O7">
+        <v>8.7422798816257696E-2</v>
+      </c>
+      <c r="P7">
+        <v>0.67</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>2500</v>
+      </c>
+      <c r="E8">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.31020527703066397</v>
+      </c>
+      <c r="I8">
+        <v>0.51399023298975399</v>
+      </c>
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8">
+        <v>0.97168254421894196</v>
+      </c>
+      <c r="M8">
+        <v>0.39760802433162801</v>
+      </c>
+      <c r="N8">
+        <v>2.4438202570290799</v>
+      </c>
+      <c r="O8">
+        <v>1.4532664851823999E-2</v>
+      </c>
+      <c r="P8">
+        <v>0.52</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>2500</v>
+      </c>
+      <c r="E9">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.31020527703066397</v>
+      </c>
+      <c r="I9">
+        <v>-1.00130816106874</v>
+      </c>
+      <c r="K9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9">
+        <v>0.82609176542999097</v>
+      </c>
+      <c r="M9">
+        <v>0.56305769420256602</v>
+      </c>
+      <c r="N9">
+        <v>1.4671529648483901</v>
+      </c>
+      <c r="O9">
+        <v>0.14233444869411199</v>
+      </c>
+      <c r="P9">
+        <v>0.45</v>
+      </c>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>5000</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I10">
+        <v>-0.89609148298922403</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10">
+        <v>0.48943129453324802</v>
+      </c>
+      <c r="M10">
+        <v>0.45563270191946298</v>
+      </c>
+      <c r="N10">
+        <v>1.0741794705941901</v>
+      </c>
+      <c r="O10">
+        <v>0.282742251679092</v>
+      </c>
+      <c r="P10">
+        <v>0.47</v>
+      </c>
+      <c r="Q10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>2500</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I11">
+        <v>-9.0866807619769896E-2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11">
+        <v>1.6500189491210799</v>
+      </c>
+      <c r="M11">
+        <v>0.80854390886273297</v>
+      </c>
+      <c r="N11">
+        <v>2.04072893387068</v>
+      </c>
+      <c r="O11">
+        <v>4.1277777750844201E-2</v>
+      </c>
+      <c r="P11">
+        <v>0.45</v>
+      </c>
+      <c r="Q11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>5000</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I12">
+        <v>-0.64440069279519596</v>
+      </c>
+      <c r="K12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12">
+        <v>4.8835240609481502E-2</v>
+      </c>
+      <c r="M12">
+        <v>0.44721736399159401</v>
+      </c>
+      <c r="N12">
+        <v>0.10919799753213399</v>
+      </c>
+      <c r="O12">
+        <v>0.91304544855079495</v>
+      </c>
+      <c r="P12">
+        <v>0.53</v>
+      </c>
+      <c r="Q12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>7500</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I13">
+        <v>1.46800953484466</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>2500</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I14">
+        <v>-0.45608147305647401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>7500</v>
+      </c>
+      <c r="E15">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I15">
+        <v>0.139840463527172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>7500</v>
+      </c>
+      <c r="E16">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I16">
+        <v>0.584823051537538</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>5000</v>
+      </c>
+      <c r="E17">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I17">
+        <v>0.24757344069488799</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>2500</v>
+      </c>
+      <c r="E18">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I18">
+        <v>-0.65683208954309402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>5000</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I19">
+        <v>0.85818000289513696</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>5000</v>
+      </c>
+      <c r="E20">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I20">
+        <v>-1.13577195887187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>5000</v>
+      </c>
+      <c r="E21">
+        <v>45</v>
+      </c>
+      <c r="F21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I21">
+        <v>-1.12388526578139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>7500</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I22">
+        <v>-0.56610181592959996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>5000</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I23">
+        <v>-0.51770894720777905</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>2500</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I24">
+        <v>-2.0935560939133301E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>7500</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I25">
+        <v>-0.23837393721778299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>5000</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I26">
+        <v>0.385583665743992</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I27">
+        <v>1.39459921186125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>2500</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I28">
+        <v>-1.1403346062467099</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>2500</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I29">
+        <v>0.33726264079316498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>7500</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>0.61593872151783002</v>
+      </c>
+      <c r="I30">
+        <v>8.1645976640445997E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>